<commit_message>
fixed ply layup format for some +-45deg laminates
</commit_message>
<xml_diff>
--- a/rdbc_data.xlsx
+++ b/rdbc_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\AM1PEPF00001BB8\EXCELCNV\4c812bcf-98c7-4adc-a633-4e46d2e22b0a\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE8FC8C9-0C00-40C7-8EA3-970FC893898D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4294F64-B7B8-4600-A1EA-A140EB3A682A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{7B04542D-A5DE-4F07-9C0B-3D89309A5622}"/>
   </bookViews>
@@ -1062,7 +1062,7 @@
     <t>reference quasi-static loading rate is too high for comparison with other collected data</t>
   </si>
   <si>
-    <t>[±45]2S</t>
+    <t>[+45/-45]2S</t>
   </si>
   <si>
     <t>10 x 10 x 2.6 mm</t>
@@ -1278,7 +1278,7 @@
     <t>55-60%</t>
   </si>
   <si>
-    <t>[0,90]4S</t>
+    <t>[+45,-45]4S</t>
   </si>
   <si>
     <t>https://doi.org/10.1016/j.compscitech.2016.09.016</t>
@@ -4227,8 +4227,8 @@
   <dimension ref="A1:X1253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A467" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R477" sqref="R477"/>
+      <pane ySplit="1" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K191" sqref="K191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>